<commit_message>
PostgreSQL example using node-postgres
</commit_message>
<xml_diff>
--- a/202108_NodeJS/NodeJS.xlsx
+++ b/202108_NodeJS/NodeJS.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\202108_NodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE16213-CC50-41F6-9BB8-E5B931C83935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77C3B73-5D23-4B59-AA92-2FECD29132F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="360" windowWidth="15330" windowHeight="10890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Course1" sheetId="2" r:id="rId2"/>
     <sheet name="Course2" sheetId="4" r:id="rId3"/>
     <sheet name="FAQ" sheetId="3" r:id="rId4"/>
+    <sheet name="TimescaleDB" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="1578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="1673">
   <si>
     <t>Mục tiêu</t>
   </si>
@@ -6139,9 +6140,6 @@
     <t>Cách 5:</t>
   </si>
   <si>
-    <t>module.export = { sayHello: sayHello }</t>
-  </si>
-  <si>
     <t>Trả về 1 object literal</t>
   </si>
   <si>
@@ -9889,13 +9887,444 @@
   </si>
   <si>
     <t>Còn nhiều vấn đề mở rộng: UI/UX, client authentication, …</t>
+  </si>
+  <si>
+    <t>https://docs.timescale.com/</t>
+  </si>
+  <si>
+    <t>https://docs.timescale.com/timescaledb/latest/overview/limitations/#distributed-hypertable-limitations</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>https://www.postgresqltutorial.com/postgresql-getting-started/</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/58239607/pgadmin-package-pgadmin4-has-no-installation-candidate</t>
+  </si>
+  <si>
+    <t>https://sysadminxpert.com/install-pgadmin-4-on-ubuntu/</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1/pgadmin4/</t>
+  </si>
+  <si>
+    <t>SELECT version();</t>
+  </si>
+  <si>
+    <t>sudo -i -u postgres</t>
+  </si>
+  <si>
+    <t>psql</t>
+  </si>
+  <si>
+    <t>\q</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/pg</t>
+  </si>
+  <si>
+    <t>node-postgres</t>
+  </si>
+  <si>
+    <t>CREATE ROLE tungbui superuser;</t>
+  </si>
+  <si>
+    <t>GRANT postgres to tungbui;</t>
+  </si>
+  <si>
+    <t>createuser tungbui</t>
+  </si>
+  <si>
+    <t>// Create user tungbui</t>
+  </si>
+  <si>
+    <t>// Assign privilege to user</t>
+  </si>
+  <si>
+    <t>\q | Exit psql connection</t>
+  </si>
+  <si>
+    <t>\c | Connect to a new database</t>
+  </si>
+  <si>
+    <t>\dt | List all tables</t>
+  </si>
+  <si>
+    <t>\du | List all roles</t>
+  </si>
+  <si>
+    <t>\list | List databases</t>
+  </si>
+  <si>
+    <t>https://blog.logrocket.com/nodejs-expressjs-postgresql-crud-rest-api-example/</t>
+  </si>
+  <si>
+    <t>ALTER USER username WITH ENCRYPTED PASSWORD 'password';</t>
+  </si>
+  <si>
+    <t>ALTER USER user_name WITH PASSWORD 'new_password';</t>
+  </si>
+  <si>
+    <t>module.exports = { sayHello: sayHello }</t>
+  </si>
+  <si>
+    <t>Use CURL to test POST, PUT, DELETE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pgAdmin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – a web-based front-end to PostgreSQL database server.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>psql</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – a terminal-based front-end to PostgreSQL database server.</t>
+    </r>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>curl --data "make=Vinfast&amp;model=Fadil1.0&amp;price=25000" http://localhost:3000/car</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>curl -X PUT -d "make=Mazda" -d "model=Mazda3.0" -d "price=30000.55" http://localhost:3000/car/4</t>
+  </si>
+  <si>
+    <t>curl -X DELETE http://localhost:3000/car/4</t>
+  </si>
+  <si>
+    <t>TimescaleDB</t>
+  </si>
+  <si>
+    <t>What is time-series data?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TimescaleDB is a </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>category-defining</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>relational database</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for time-series data. Packaged as a PostgreSQL extension.</t>
+    </r>
+  </si>
+  <si>
+    <t>Time-series data is data that collectively represents how a system, process, or behavior changes over time.</t>
+  </si>
+  <si>
+    <t>Metrics: CPU, free_mem, net_rssi, battery</t>
+  </si>
+  <si>
+    <t>Tags:    Host=MyServer, Region=West</t>
+  </si>
+  <si>
+    <t>Data:</t>
+  </si>
+  <si>
+    <t>2017-01-01 01:02:00    70    500    -40    80</t>
+  </si>
+  <si>
+    <t>2017-01-01 01:03:00    71    400    -42    80</t>
+  </si>
+  <si>
+    <t>2017-01-01 01:04:00    72    367    -41    80</t>
+  </si>
+  <si>
+    <t>2017-01-01 01:05:01    68    750    -54    79</t>
+  </si>
+  <si>
+    <t>Characteristics of time-series data</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Time-centric</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>Data record luôn có một timestamp</t>
+  </si>
+  <si>
+    <t>Append-only:</t>
+  </si>
+  <si>
+    <t>Data hầu hết là được append (INSERTs)</t>
+  </si>
+  <si>
+    <t>Recent:</t>
+  </si>
+  <si>
+    <t>New data thường là của time interval mới nhất, chúng ta rất hiếm khi update hoặc backfill missing data của interval cũ.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Key difference giữa time-series data và các loại data khác đó là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>thay đổi data là insert chứ ko overwrite.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hypertables</t>
+  </si>
+  <si>
+    <t>Điểm để tương tác với dữ liệu, cung cấp abstraction của bảng tiêu chuẩn có thể query qua standard SQL.</t>
+  </si>
+  <si>
+    <t>Ví dụ: tạo một hypertable</t>
+  </si>
+  <si>
+    <t>CREATE TABLE (with standard SQL syntax)</t>
+  </si>
+  <si>
+    <t>SELECT create_hypertable()</t>
+  </si>
+  <si>
+    <t>Một cách trừu tượng thì các tương tác của user với TimescaleDB là với hypertable (insert, update, delete, query, altering, …).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tuy nhiên, hypertables thực chất là một abstraction hay virtual view của rất nhiều bảng chứa data, gọi là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chunks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Partitioning in hypertables with chunks</t>
+  </si>
+  <si>
+    <t>Chunk được tạo bằng cách phân mảnh một hypertable's data thành một hoặc nhiều chiều.</t>
+  </si>
+  <si>
+    <t>Ví dụ, nếu phân mảnh thời gian theo quãng 1 ngày, các row với timestamp cùng ngày được đặt vào cùng một chunk.</t>
+  </si>
+  <si>
+    <t>Tất cả hypertables được phân mảnh theo giá trị của time column (vd: timestamp, date, …)</t>
+  </si>
+  <si>
+    <t>TimescaleDB tự động tạo các chunk khi row được insert vào DB.</t>
+  </si>
+  <si>
+    <t>Một hypertable có thể được phân mảnh thêm theo các cột khác, ví dụ device id, location, user id, …</t>
+  </si>
+  <si>
+    <t>Gọi là phân mảnh "time-and-space" - được dùng chủ yếu cho distributed hypertables.</t>
+  </si>
+  <si>
+    <t>Scaling TimescaleDB</t>
+  </si>
+  <si>
+    <t>TimescaleDB hỗ trợ 3 lựa chọn triển khai:</t>
+  </si>
+  <si>
+    <t>an single DB server</t>
+  </si>
+  <si>
+    <t>a traditional primary/replica deployment</t>
+  </si>
+  <si>
+    <t>a multi-node deployment with horizontal scalability</t>
+  </si>
+  <si>
+    <t>Phần mềm Node Todos!</t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách các công việc todos cần làm</t>
+  </si>
+  <si>
+    <t>REQ 1</t>
+  </si>
+  <si>
+    <t>REQ 2</t>
+  </si>
+  <si>
+    <t>Có thể thêm mới một đầu việc todo (INSERT)</t>
+  </si>
+  <si>
+    <t>REQ 3</t>
+  </si>
+  <si>
+    <t>Có thể sửa/cập nhật nội dung một đầu việc todo (UPDATE)</t>
+  </si>
+  <si>
+    <t>REQ 4</t>
+  </si>
+  <si>
+    <t>Mỗi một todo có thể được đánh dấu trạng thái là hoàn thành 'done'</t>
+  </si>
+  <si>
+    <t>REQ 5</t>
+  </si>
+  <si>
+    <t>Có thể xóa được một đầu việc todo (DELETE)</t>
+  </si>
+  <si>
+    <t>Các thư viện NPM</t>
+  </si>
+  <si>
+    <t>express</t>
+  </si>
+  <si>
+    <t>ejs</t>
+  </si>
+  <si>
+    <t>body-parser</t>
+  </si>
+  <si>
+    <t>morgan</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>PostgreSQL DB client</t>
+  </si>
+  <si>
+    <t>Views support</t>
+  </si>
+  <si>
+    <t>RESTful API support</t>
+  </si>
+  <si>
+    <t>Logging support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10158,6 +10587,16 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -14822,7 +15261,7 @@
   <dimension ref="B2:O46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15391,7 +15830,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N105" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -16798,10 +17237,10 @@
         <v>88</v>
       </c>
       <c r="I379" s="6" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="M379" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="380" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -16822,10 +17261,10 @@
     </row>
     <row r="383" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I383" s="6" t="s">
+        <v>1320</v>
+      </c>
+      <c r="M383" t="s">
         <v>1321</v>
-      </c>
-      <c r="M383" t="s">
-        <v>1322</v>
       </c>
     </row>
     <row r="384" spans="2:13" x14ac:dyDescent="0.25">
@@ -16845,7 +17284,7 @@
     </row>
     <row r="388" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C388" s="2" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F388" t="s">
         <v>504</v>
@@ -16854,7 +17293,7 @@
         <v>529</v>
       </c>
       <c r="U388" s="6" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="389" spans="2:21" x14ac:dyDescent="0.25">
@@ -16870,7 +17309,7 @@
     </row>
     <row r="390" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C390" s="2" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="F390" t="s">
         <v>505</v>
@@ -16907,7 +17346,7 @@
         <v>525</v>
       </c>
       <c r="U393" s="6" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="394" spans="2:21" x14ac:dyDescent="0.25">
@@ -16966,7 +17405,7 @@
         <v>513</v>
       </c>
       <c r="O398" s="6" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="U398" s="6" t="s">
         <v>540</v>
@@ -17591,10 +18030,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB349D5-341F-411C-BD3F-ECBC2645FBB8}">
-  <dimension ref="A2:U664"/>
+  <dimension ref="A2:U682"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A620" workbookViewId="0">
-      <selection activeCell="F643" sqref="F643"/>
+    <sheetView tabSelected="1" topLeftCell="A641" workbookViewId="0">
+      <selection activeCell="E668" sqref="E668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17609,7 +18048,7 @@
         <v>856</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -17617,7 +18056,7 @@
         <v>857</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -17933,7 +18372,7 @@
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C67" s="24" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="N67" t="s">
         <v>912</v>
@@ -17941,7 +18380,7 @@
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C68" s="24" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="N68" t="s">
         <v>908</v>
@@ -17971,7 +18410,7 @@
         <v>909</v>
       </c>
       <c r="S71" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
@@ -18023,10 +18462,10 @@
         <v>923</v>
       </c>
       <c r="N81" t="s">
+        <v>1104</v>
+      </c>
+      <c r="T81" t="s">
         <v>1105</v>
-      </c>
-      <c r="T81" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="82" spans="2:20" x14ac:dyDescent="0.25">
@@ -18086,7 +18525,7 @@
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.25">
@@ -18137,7 +18576,7 @@
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D108" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I108" s="6" t="s">
         <v>939</v>
@@ -18249,44 +18688,44 @@
         <v>968</v>
       </c>
       <c r="D120" s="6" t="s">
+        <v>1604</v>
+      </c>
+      <c r="I120" t="s">
         <v>969</v>
-      </c>
-      <c r="I120" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="123" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="J124" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D125" s="6" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K125" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D126" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="K126" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="127" spans="2:12" x14ac:dyDescent="0.25">
@@ -18299,43 +18738,43 @@
     </row>
     <row r="128" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D128" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="K128" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="129" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D129" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="K129" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C132" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="134" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="136" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="137" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C137" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="H137" s="6" t="s">
         <v>887</v>
@@ -18346,25 +18785,25 @@
         <v>941</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C139" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H139" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C140" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="141" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C141" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="142" spans="2:11" x14ac:dyDescent="0.25">
@@ -18374,41 +18813,41 @@
     </row>
     <row r="145" spans="1:8" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="23" t="s">
+        <v>985</v>
+      </c>
+      <c r="C145" s="23" t="s">
         <v>986</v>
-      </c>
-      <c r="C145" s="23" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F150" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F151" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -18418,43 +18857,43 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C154" s="6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C155" s="6" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C156" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C159" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C160" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="H160" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="161" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C161" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="H161" s="6" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="162" spans="2:15" x14ac:dyDescent="0.25">
@@ -18467,32 +18906,32 @@
     </row>
     <row r="163" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C163" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="165" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="166" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="167" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C167" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="168" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C168" s="3" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="169" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D169" s="6" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="K169" t="s">
         <v>887</v>
@@ -18500,10 +18939,10 @@
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D170" s="6" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="K170" s="6" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="171" spans="2:15" x14ac:dyDescent="0.25">
@@ -18511,32 +18950,32 @@
         <v>46</v>
       </c>
       <c r="K171" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="O171" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="172" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D172" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="K172" s="6"/>
     </row>
     <row r="173" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D173" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="K173" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D174" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="K174" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
@@ -18549,40 +18988,40 @@
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D176" s="6" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="K176" s="6"/>
     </row>
     <row r="177" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D177" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="K177" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="178" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D178" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="K178" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="179" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D179" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="K179" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="180" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D180" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="K180" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="181" spans="2:12" x14ac:dyDescent="0.25">
@@ -18590,7 +19029,7 @@
         <v>353</v>
       </c>
       <c r="K181" s="6" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="182" spans="2:12" x14ac:dyDescent="0.25">
@@ -18603,7 +19042,7 @@
     </row>
     <row r="183" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D183" s="6" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="K183" s="6" t="s">
         <v>46</v>
@@ -18611,54 +19050,54 @@
     </row>
     <row r="185" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="186" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C186" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="187" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D187" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L187" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="188" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D188" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="L188" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="189" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D189" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L189" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="190" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D190" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="L190" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="191" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D191" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="192" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D192" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="193" spans="2:10" x14ac:dyDescent="0.25">
@@ -18668,52 +19107,52 @@
     </row>
     <row r="195" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="196" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C196" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="197" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C197" s="24" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="198" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D198" s="6" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="J198" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="199" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D199" s="6" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="J199" s="6" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="200" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D200" s="6"/>
       <c r="J200" s="6" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="201" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D201" s="6" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="J201" s="6" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="202" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D202" s="6" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="J202" s="6" t="s">
         <v>46</v>
@@ -18727,20 +19166,20 @@
     </row>
     <row r="204" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D204" s="25" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="J204" s="6" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="205" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J205" s="6" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="206" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J206" s="6" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="207" spans="2:10" x14ac:dyDescent="0.25">
@@ -18750,97 +19189,97 @@
     </row>
     <row r="208" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J208" s="6" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="210" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="211" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="212" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F212" s="6" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="213" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F213" s="6" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="214" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F214" s="6" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="216" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="217" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C217" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="218" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C218" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="219" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C219" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="220" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D220" s="6" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="221" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D221" s="6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J221" s="6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="222" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D222" s="6" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J222" s="6" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="223" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D223" s="6" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="J223" s="6" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="224" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D224" s="6" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D225" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
@@ -18850,82 +19289,82 @@
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C229" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C232" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D233" s="6" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D234" s="6" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D235" s="6" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D236" s="6" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D237" s="6" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C240" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D241" s="6" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D242" s="6" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D243" s="6" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D244" s="6" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D245" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -18940,10 +19379,10 @@
     </row>
     <row r="250" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="8" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -18953,230 +19392,230 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C253" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C254" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="257" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C257" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="258" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C258" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="260" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K260" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="N260" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="261" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="262" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C262" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="264" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="265" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C265" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D265" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="266" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D266" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="267" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C267" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D267" t="s">
         <v>1119</v>
-      </c>
-      <c r="D267" t="s">
-        <v>1120</v>
       </c>
     </row>
     <row r="268" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D268" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="270" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="271" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C271" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="272" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C272" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C275" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D276" s="6" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="277" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D277" s="6" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="278" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D278" s="6" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D279" s="6" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D280" s="6" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="281" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D281" s="6" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="283" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D283" s="6" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D284" s="6" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="286" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="287" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C287" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C288" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="289" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C289" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D290" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="291" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D291" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="292" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D292" s="6" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="293" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D293" s="6" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="294" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D294" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="295" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D295" s="6" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="297" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="298" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C298" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="I298" s="6" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="299" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C299" s="6" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="I299" s="6" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="300" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C300" s="6" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="I300" s="6" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="301" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C301" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="302" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C302" s="6" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="303" spans="2:9" x14ac:dyDescent="0.25">
@@ -19186,48 +19625,48 @@
     </row>
     <row r="305" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="306" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C306" s="18" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E306" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="307" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C307" s="18" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E307" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="308" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C308" s="6"/>
       <c r="D308" s="6" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="309" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C309" s="6"/>
       <c r="D309" s="6" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="310" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D310" s="6" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="K310" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="311" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D311" s="6" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="312" spans="2:11" x14ac:dyDescent="0.25">
@@ -19237,45 +19676,45 @@
     </row>
     <row r="314" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="315" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C315" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D315" s="3" t="s">
         <v>1159</v>
-      </c>
-      <c r="D315" s="3" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="316" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D316" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="317" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D317" s="3" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="319" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C319" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="320" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D320" s="6" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="321" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D321" s="6" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="322" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D322" s="6" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="323" spans="2:14" x14ac:dyDescent="0.25">
@@ -19285,22 +19724,22 @@
     </row>
     <row r="324" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D324" s="6" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="325" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D325" s="6" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="326" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D326" s="6" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="327" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D327" s="6" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="328" spans="2:14" x14ac:dyDescent="0.25">
@@ -19310,392 +19749,392 @@
     </row>
     <row r="331" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="332" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C332" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="333" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C333" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="334" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C334" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="335" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C335" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="336" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J336" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="N336" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C339" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D340" s="6" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D341" s="6" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D342" s="6" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C343" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D344" s="6" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="348" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="8" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C348" s="8" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C351" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C352" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="354" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="355" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C355" t="s">
+        <v>1225</v>
+      </c>
+      <c r="P355" t="s">
         <v>1226</v>
-      </c>
-      <c r="P355" t="s">
-        <v>1227</v>
       </c>
     </row>
     <row r="356" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C356" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F356" t="s">
         <v>1222</v>
       </c>
-      <c r="F356" t="s">
+      <c r="G356" t="s">
         <v>1223</v>
-      </c>
-      <c r="G356" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="357" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F357" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="G357" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="359" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G359" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="361" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G361" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="363" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="364" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C364" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="365" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C365" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="366" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C366" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="368" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="369" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C369" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="370" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C370" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="371" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C371" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="372" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C372" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="374" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="375" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C375" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="376" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C376" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="377" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C377" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="378" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C378" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="379" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C379" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="380" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D380" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="381" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E381" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="382" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C382" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="I382" s="2" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="383" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D383" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="J383" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="384" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D384" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="J384" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="385" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D385" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="J385" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="386" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J386" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="387" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J387" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="389" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C389" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="390" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C390" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="391" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C391" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="393" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C393" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="395" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="396" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C396" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="398" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="399" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C399" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="400" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D400" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="401" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D401" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="402" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D402" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="403" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D403" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="404" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D404" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="405" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C405" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="406" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C406" s="1" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="408" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="409" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C409" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="410" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D410" s="6" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="411" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D411" s="6" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="412" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D412" s="6" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="413" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D413" s="6" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="414" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D414" s="6" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="415" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D415" s="6" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="417" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="418" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C418" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="419" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C419" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="420" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D420" s="6" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="L420" s="6" t="s">
         <v>887</v>
@@ -19703,181 +20142,181 @@
     </row>
     <row r="421" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D421" s="6" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="L421" s="6" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="422" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D422" s="6" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="L422" s="6" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="423" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D423" s="6" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="L423" s="6" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="424" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D424" s="6" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="L424" s="6" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="425" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D425" s="6" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="L425" s="6" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="426" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D426" s="6" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="G426" s="24" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="L426" s="6" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="427" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D427" s="6" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="L427" s="6" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="428" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D428" s="6" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="430" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="431" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C431" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="432" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C432" s="26" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="433" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C433" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="434" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D434" s="6" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="435" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D435" s="6" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="436" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D436" s="6" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="437" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D437" s="6" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="439" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="440" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C440" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="441" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C441" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="443" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="444" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C444" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="445" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C445" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="446" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D446" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="447" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C447" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C450" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D451" s="6" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D452" s="6" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D453" s="6" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="454" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D454" s="6" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="455" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D455" s="6" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="456" spans="2:4" x14ac:dyDescent="0.25">
@@ -19887,67 +20326,67 @@
     </row>
     <row r="457" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D457" s="6" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="458" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D458" s="6" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="460" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="461" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C461" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="462" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C462" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="463" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C463" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="464" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C464" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D465" s="6" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D466" s="6" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D467" s="6" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D468" s="6" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D469" s="6" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D470" s="6" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
@@ -19957,12 +20396,12 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D472" s="6" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D473" s="6" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
@@ -19972,110 +20411,110 @@
     </row>
     <row r="477" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A477" s="8" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C477" s="8" t="s">
         <v>1299</v>
-      </c>
-      <c r="C477" s="8" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C480" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="481" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C481" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="483" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B483" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="484" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C484" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="486" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B486" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="487" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C487" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="488" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C488" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="489" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C489" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="491" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B491" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="492" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C492" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="493" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C493" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="494" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C494" s="4" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="495" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D495" s="33" t="s">
+        <v>1323</v>
+      </c>
+      <c r="H495" t="s">
         <v>1324</v>
       </c>
-      <c r="H495" t="s">
+      <c r="I495" t="s">
         <v>1325</v>
-      </c>
-      <c r="I495" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="496" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H496" t="s">
+        <v>1326</v>
+      </c>
+      <c r="I496" t="s">
         <v>1327</v>
-      </c>
-      <c r="I496" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="497" spans="2:20" x14ac:dyDescent="0.25">
       <c r="H497" t="s">
+        <v>1328</v>
+      </c>
+      <c r="I497" t="s">
         <v>1329</v>
-      </c>
-      <c r="I497" t="s">
-        <v>1330</v>
       </c>
     </row>
     <row r="499" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="N499" s="6" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="500" spans="2:20" x14ac:dyDescent="0.25">
@@ -20091,152 +20530,152 @@
         <v>87</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="N501" s="6" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="502" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D502" s="6" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="G502" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="N502" s="6" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="503" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C503" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="N503" s="6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="504" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D504" s="6" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="N504" s="6" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="505" spans="2:20" x14ac:dyDescent="0.25">
       <c r="N505" s="6" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="506" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="N506" s="6" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="T506" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="507" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C507" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="N507" s="6" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="T507" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="508" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C508" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="N508" s="6" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="509" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D509" s="6" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F509" t="s">
         <v>1338</v>
       </c>
-      <c r="F509" t="s">
-        <v>1339</v>
-      </c>
       <c r="N509" s="6" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="510" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C510" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="N510" s="6" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="511" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D511" s="6" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="N511" s="6" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="T511" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="512" spans="2:20" x14ac:dyDescent="0.25">
       <c r="N512" s="6" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="513" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B513" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="N513" s="6" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="514" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C514" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="N514" s="6" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="T514" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="515" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N515" s="6" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="516" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B516" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="N516" s="6" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="517" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C517" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="N517" s="6" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="518" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D518" s="6" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="N518" s="6" t="s">
         <v>354</v>
@@ -20244,7 +20683,7 @@
     </row>
     <row r="519" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D519" s="6" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="N519" s="6" t="s">
         <v>46</v>
@@ -20252,20 +20691,20 @@
     </row>
     <row r="523" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A523" s="8" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="C523" s="8" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="525" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B525" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="526" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C526" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="N526" s="6" t="s">
         <v>887</v>
@@ -20273,45 +20712,45 @@
     </row>
     <row r="527" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C527" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="N527" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="528" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D528" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="N528" s="6" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="529" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N529" s="6" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="530" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B530" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="N530" s="6"/>
     </row>
     <row r="531" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C531" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="N531" s="6" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="532" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C532" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="N532" s="6" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="533" spans="2:14" x14ac:dyDescent="0.25">
@@ -20321,32 +20760,32 @@
     </row>
     <row r="534" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B534" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="N534" s="6"/>
     </row>
     <row r="535" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C535" s="1" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="N535" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="536" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D536" t="s">
+        <v>1392</v>
+      </c>
+      <c r="F536" t="s">
         <v>1393</v>
       </c>
-      <c r="F536" t="s">
-        <v>1394</v>
-      </c>
       <c r="N536" s="6" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="537" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D537" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="N537" s="6" t="s">
         <v>385</v>
@@ -20354,39 +20793,39 @@
     </row>
     <row r="538" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D538" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="539" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D539" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="N539" s="6" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="540" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D540" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F540" t="s">
         <v>1398</v>
       </c>
-      <c r="F540" t="s">
-        <v>1399</v>
-      </c>
       <c r="N540" s="6" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="541" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D541" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="N541" s="6" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="542" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D542" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="N542" s="6" t="s">
         <v>385</v>
@@ -20394,73 +20833,73 @@
     </row>
     <row r="544" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B544" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="545" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C545" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="546" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C546" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="548" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B548" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="N548" s="6" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="549" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C549" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="N549" s="6" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="U549" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="550" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C550" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="N550" s="6" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="551" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C551" s="24" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="N551" s="6" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="552" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C552" s="24" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="N552" s="6" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="U552" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="553" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N553" s="6" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="554" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N554" s="6" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="555" spans="2:21" x14ac:dyDescent="0.25">
@@ -20470,42 +20909,42 @@
     </row>
     <row r="557" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B557" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="558" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C558" t="s">
+        <v>1418</v>
+      </c>
+      <c r="N558" s="6" t="s">
         <v>1419</v>
       </c>
-      <c r="N558" s="6" t="s">
-        <v>1420</v>
-      </c>
       <c r="S558" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="559" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C559" s="24" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="N559" s="6" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="S559" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="560" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N560" s="6" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="S560" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="561" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N561" s="18" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="562" spans="2:19" x14ac:dyDescent="0.25">
@@ -20515,12 +20954,12 @@
     </row>
     <row r="564" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B564" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="565" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C565" s="1" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="N565" s="6" t="s">
         <v>887</v>
@@ -20528,46 +20967,46 @@
     </row>
     <row r="566" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C566" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="N566" s="6" t="s">
+        <v>1437</v>
+      </c>
+      <c r="S566" t="s">
         <v>1438</v>
-      </c>
-      <c r="S566" t="s">
-        <v>1439</v>
       </c>
     </row>
     <row r="567" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C567" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="N567" s="6"/>
       <c r="S567" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="568" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D568" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="N568" s="6" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="569" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C569" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="N569" s="6" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="S569" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="570" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C570" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="N570" s="6" t="s">
         <v>385</v>
@@ -20575,25 +21014,25 @@
     </row>
     <row r="571" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D571" s="6" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="572" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N572" s="6" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="573" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N573" s="6" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="574" spans="2:19" x14ac:dyDescent="0.25">
       <c r="N574" s="6" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="S574" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="575" spans="2:19" x14ac:dyDescent="0.25">
@@ -20603,75 +21042,75 @@
     </row>
     <row r="577" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B577" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="G577" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J577" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="578" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C578" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="579" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D579" t="s">
+        <v>1451</v>
+      </c>
+      <c r="M579" t="s">
         <v>1452</v>
-      </c>
-      <c r="M579" t="s">
-        <v>1453</v>
       </c>
     </row>
     <row r="580" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D580" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="M580" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="581" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D581" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="M581" s="34" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="582" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D582" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="M582" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="583" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M583" s="34" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="585" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C585" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="586" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D586" s="6" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="587" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D587" s="6" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="588" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D588" s="6" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="589" spans="2:13" x14ac:dyDescent="0.25">
@@ -20681,38 +21120,38 @@
     </row>
     <row r="591" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C591" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="M591" s="6" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="592" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D592" s="6" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="M592" s="6" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="593" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M593" s="6" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="594" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M594" s="6" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="595" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M595" s="6" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="596" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M596" s="6" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="597" spans="2:13" x14ac:dyDescent="0.25">
@@ -20722,242 +21161,470 @@
     </row>
     <row r="599" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B599" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="600" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C600" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="601" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C601" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="602" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C602" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="604" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B604" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="605" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C605" s="1" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="606" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C606" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="607" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D607" s="6" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="608" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D608" s="6" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D609" s="6" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D610" s="6" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="614" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A614" s="8" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="C614" s="8" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B616" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C617" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D618" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E619" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E620" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D621" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D622" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B624" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="625" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C625" t="s">
         <v>1546</v>
       </c>
-    </row>
-    <row r="625" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C625" t="s">
+      <c r="L625" s="2" t="s">
+        <v>1551</v>
+      </c>
+      <c r="N625" s="2" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="626" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C626" s="1" t="s">
         <v>1547</v>
       </c>
-      <c r="L625" s="2" t="s">
+      <c r="L626" t="s">
+        <v>1553</v>
+      </c>
+      <c r="N626" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="627" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L627" t="s">
+        <v>1554</v>
+      </c>
+      <c r="N627" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="628" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B628" t="s">
+        <v>1548</v>
+      </c>
+      <c r="L628" t="s">
+        <v>1555</v>
+      </c>
+      <c r="N628" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="629" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C629" t="s">
+        <v>1549</v>
+      </c>
+      <c r="L629" t="s">
+        <v>1556</v>
+      </c>
+      <c r="N629" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="630" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C630" t="s">
+        <v>1550</v>
+      </c>
+      <c r="L630" t="s">
+        <v>1557</v>
+      </c>
+      <c r="N630" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="631" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C631" t="s">
+        <v>1565</v>
+      </c>
+      <c r="L631" t="s">
+        <v>1558</v>
+      </c>
+      <c r="N631" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="633" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B633" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="635" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B635" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="636" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C636" s="1" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="637" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D637" t="s">
+        <v>1607</v>
+      </c>
+      <c r="N637" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="638" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D638" t="s">
+        <v>1606</v>
+      </c>
+      <c r="N638" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="639" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C639" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="N639" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="640" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C640" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="N640" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="641" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D641" s="1" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="642" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D642" t="s">
+        <v>1584</v>
+      </c>
+      <c r="N642" t="s">
+        <v>1593</v>
+      </c>
+      <c r="R642" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="643" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N643" t="s">
+        <v>1591</v>
+      </c>
+      <c r="R643" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="644" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C644" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="N644" t="s">
+        <v>1592</v>
+      </c>
+      <c r="R644" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="645" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C645" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E645" s="1" t="s">
+        <v>1589</v>
+      </c>
+      <c r="N645" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="646" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C646" t="s">
+        <v>1605</v>
+      </c>
+      <c r="N646" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="647" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D647" t="s">
+        <v>1608</v>
+      </c>
+      <c r="E647" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="648" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D648" t="s">
+        <v>1610</v>
+      </c>
+      <c r="E648" t="s">
+        <v>1612</v>
+      </c>
+      <c r="O648" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="649" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D649" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E649" t="s">
+        <v>1613</v>
+      </c>
+      <c r="O649" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="650" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O650" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="651" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O651" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="652" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O652" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="655" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A655" s="8" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C655" s="8" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="657" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B657" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="658" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C658" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D658" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="659" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C659" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D659" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="660" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C660" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D660" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="661" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C661" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D661" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="662" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C662" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D662" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="664" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B664" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="665" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C665" t="s">
+        <v>1664</v>
+      </c>
+      <c r="E665" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="666" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C666" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="667" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C667" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E667" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="668" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C668" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E668" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="669" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C669" t="s">
+        <v>1668</v>
+      </c>
+      <c r="E669" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="674" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A674" s="8" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C674" s="8" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="676" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B676" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E676" t="s">
+        <v>870</v>
+      </c>
+      <c r="G676" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="677" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H677" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="678" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E678" t="s">
+        <v>868</v>
+      </c>
+      <c r="G678" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="679" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H679" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="680" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E680" t="s">
+        <v>1553</v>
+      </c>
+      <c r="G680" t="s">
         <v>1552</v>
       </c>
-      <c r="N625" s="2" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="626" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C626" s="1" t="s">
-        <v>1548</v>
-      </c>
-      <c r="L626" t="s">
-        <v>1554</v>
-      </c>
-      <c r="N626" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="627" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L627" t="s">
-        <v>1555</v>
-      </c>
-      <c r="N627" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="628" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B628" t="s">
-        <v>1549</v>
-      </c>
-      <c r="L628" t="s">
-        <v>1556</v>
-      </c>
-      <c r="N628" t="s">
-        <v>1561</v>
-      </c>
-    </row>
-    <row r="629" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C629" t="s">
-        <v>1550</v>
-      </c>
-      <c r="L629" t="s">
-        <v>1557</v>
-      </c>
-      <c r="N629" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="630" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C630" t="s">
-        <v>1551</v>
-      </c>
-      <c r="L630" t="s">
-        <v>1558</v>
-      </c>
-      <c r="N630" t="s">
-        <v>1563</v>
-      </c>
-    </row>
-    <row r="631" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C631" t="s">
-        <v>1566</v>
-      </c>
-      <c r="L631" t="s">
-        <v>1559</v>
-      </c>
-      <c r="N631" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="633" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B633" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="637" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A637" s="8" t="s">
-        <v>1569</v>
-      </c>
-      <c r="C637" s="8" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="656" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A656" s="8" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C656" s="8" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="658" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B658" t="s">
-        <v>1572</v>
-      </c>
-      <c r="E658" t="s">
-        <v>870</v>
-      </c>
-      <c r="G658" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="659" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H659" t="s">
+    </row>
+    <row r="682" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B682" t="s">
         <v>1576</v>
-      </c>
-    </row>
-    <row r="660" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E660" t="s">
-        <v>868</v>
-      </c>
-      <c r="G660" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="661" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H661" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="662" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E662" t="s">
-        <v>1554</v>
-      </c>
-      <c r="G662" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="664" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B664" t="s">
-        <v>1577</v>
       </c>
     </row>
   </sheetData>
@@ -20975,9 +21642,15 @@
     <hyperlink ref="C565" r:id="rId11" xr:uid="{8036714D-F280-431A-B6FA-2BB1C74E5098}"/>
     <hyperlink ref="C605" r:id="rId12" xr:uid="{687F245F-B1FA-47A9-B034-0968F369AFB5}"/>
     <hyperlink ref="C626" r:id="rId13" xr:uid="{39ADBE7F-6A12-4219-A28A-698ED475DB2E}"/>
+    <hyperlink ref="C636" r:id="rId14" xr:uid="{9FB45DEC-F041-4FEA-B876-A0ED7680E3CF}"/>
+    <hyperlink ref="C639" r:id="rId15" xr:uid="{4EBD8767-8DE2-47A8-BCD0-934C15CBDB6A}"/>
+    <hyperlink ref="C640" r:id="rId16" xr:uid="{63EFBE9C-B788-4B84-8A87-6F75DF52346C}"/>
+    <hyperlink ref="D641" r:id="rId17" xr:uid="{AF42B8EA-677E-45AC-8CFE-0C8ECFE62FC7}"/>
+    <hyperlink ref="C644" r:id="rId18" xr:uid="{31C7B9F4-F505-472C-934C-076A6FA73585}"/>
+    <hyperlink ref="E645" r:id="rId19" xr:uid="{68187904-D8EB-417C-8159-14220E107848}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -21063,7 +21736,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="21" spans="2:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -22572,269 +23245,269 @@
     </row>
     <row r="366" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B366" s="8" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="367" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B367" s="1" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="368" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B368" s="1" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="369" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="370" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C370" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="371" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C371" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="372" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C372" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="373" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D373" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="E373" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="G373" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="374" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E374" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="G374" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="376" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="377" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C377" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="378" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D378" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="379" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D379" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="380" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E380" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="381" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D381" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="382" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D382" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="383" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D383" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="384" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D384" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="386" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C386" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="387" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C387" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="388" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C388" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="390" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="391" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C391" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="392" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D392" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="393" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C393" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="394" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D394" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="395" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C395" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="396" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C396" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="397" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D397" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="398" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D398" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="399" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C399" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="400" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C400" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="401" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D401" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="402" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C402" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="403" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D403" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="404" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D404" s="35" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="406" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="407" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C407" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="408" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C408" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="409" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C409" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="410" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D410" s="6" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="411" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D411" s="6" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="I411" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="M411" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="412" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D412" s="6" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="I412" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="M412" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="413" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D413" s="6" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="414" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D414" s="6" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="415" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D415" s="6" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="I415" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="M415" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="416" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D416" s="6" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="417" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D417" s="6" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="418" spans="4:4" x14ac:dyDescent="0.25">
@@ -22858,4 +23531,217 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
   <drawing r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65A888-D5D2-4251-A9B3-6660522D7653}">
+  <dimension ref="B2:E44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="19" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>1626</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>1628</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C482E7A7-C9CC-4CCF-9FB8-EB8ECF0B12C5}"/>
+    <hyperlink ref="B3" r:id="rId2" location="distributed-hypertable-limitations" xr:uid="{F533ED10-9B5D-40CD-BD46-40FFA8121591}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>